<commit_message>
Added Joe Garcia's code
</commit_message>
<xml_diff>
--- a/Project 5 Master Document.xlsx
+++ b/Project 5 Master Document.xlsx
@@ -6,6 +6,7 @@
     <sheet state="visible" name="Team Members" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Team Artifacts" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Project Activities" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Data Tables" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="96">
   <si>
     <t>Team Member</t>
   </si>
@@ -27,12 +28,6 @@
     <t>peiming.chen94@spsmail.cuny.edu</t>
   </si>
   <si>
-    <t>Daniel Craig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dcraig4991@gmail.com </t>
-  </si>
-  <si>
     <t>Genesis Middleton</t>
   </si>
   <si>
@@ -123,54 +118,51 @@
     <t>Develop Entity Relationships for Database</t>
   </si>
   <si>
+    <t>Entity Relationship diagram</t>
+  </si>
+  <si>
+    <t>Write project overview document</t>
+  </si>
+  <si>
+    <t>Project Overview document</t>
+  </si>
+  <si>
+    <t>Share document with team for review</t>
+  </si>
+  <si>
+    <t>Team provides edits and comments on document</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Submit document</t>
+  </si>
+  <si>
+    <t>Part 2 - Data Analysis</t>
+  </si>
+  <si>
+    <t>Data Collection</t>
+  </si>
+  <si>
+    <t>Create spreadsheet to use for data dump</t>
+  </si>
+  <si>
+    <t>Job Postings Spreadsheet</t>
+  </si>
+  <si>
+    <t>Scrape assigned websites for job postings and paste into shared Google Sheet</t>
+  </si>
+  <si>
     <t>Not Started</t>
   </si>
   <si>
-    <t>Entity Relationship diagram</t>
-  </si>
-  <si>
-    <t>Write project overview document</t>
-  </si>
-  <si>
-    <t>Project Overview document</t>
-  </si>
-  <si>
-    <t>Share document with team for review</t>
-  </si>
-  <si>
-    <t>Team provides edits and comments on document</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Submit document</t>
-  </si>
-  <si>
-    <t>Part 2 - Data Analysis</t>
-  </si>
-  <si>
-    <t>Data Collection</t>
-  </si>
-  <si>
-    <t>Create spreadsheet to use for data dump</t>
-  </si>
-  <si>
-    <t>Job Postings Spreadsheet</t>
-  </si>
-  <si>
-    <t>Scrape assigned websites for job postings and paste into shared Google Sheet</t>
-  </si>
-  <si>
     <t>Completed job posting spreadsheet</t>
   </si>
   <si>
     <t>Setup database and data tables in AWS</t>
   </si>
   <si>
-    <t>Genesis / Daniel</t>
-  </si>
-  <si>
     <t>Database setup in AWS</t>
   </si>
   <si>
@@ -198,7 +190,7 @@
     <t>Analysis of data</t>
   </si>
   <si>
-    <t>PeiMing / Daniel / ?</t>
+    <t>PeiMing</t>
   </si>
   <si>
     <t>Code for analyzing data and creating data visualizations</t>
@@ -220,7 +212,7 @@
     <t>Create individual content slides</t>
   </si>
   <si>
-    <t>Kory, Genesis, Joe, Daniel</t>
+    <t>Kory, Genesis, Joe,</t>
   </si>
   <si>
     <t>Complete indeividual slides</t>
@@ -229,7 +221,7 @@
     <t>Finalize slides</t>
   </si>
   <si>
-    <t>Daniel</t>
+    <t>Kory / Genesis</t>
   </si>
   <si>
     <t>Completed presentation deck</t>
@@ -239,6 +231,78 @@
   </si>
   <si>
     <t>Team Presentation</t>
+  </si>
+  <si>
+    <t>Kory, Genesis, Joe</t>
+  </si>
+  <si>
+    <t>job_board</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>job_board_name</t>
+  </si>
+  <si>
+    <t>var char</t>
+  </si>
+  <si>
+    <t>company_name</t>
+  </si>
+  <si>
+    <t>posting_id</t>
+  </si>
+  <si>
+    <t>job_board_url</t>
+  </si>
+  <si>
+    <t>company_location</t>
+  </si>
+  <si>
+    <t>skill_name</t>
+  </si>
+  <si>
+    <t>industry</t>
+  </si>
+  <si>
+    <t>skill_type</t>
+  </si>
+  <si>
+    <t>posting</t>
+  </si>
+  <si>
+    <t>company_id</t>
+  </si>
+  <si>
+    <t>job_board_id</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>industry_name</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>senority_level</t>
+  </si>
+  <si>
+    <t>work_type</t>
+  </si>
+  <si>
+    <t>min_years_experience</t>
   </si>
 </sst>
 </file>
@@ -248,7 +312,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -270,8 +334,9 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font/>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,8 +379,14 @@
         <bgColor rgb="FFC9DAF8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border/>
     <border>
       <left style="thin">
@@ -331,11 +402,33 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -457,6 +550,19 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="2" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -474,6 +580,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -725,14 +835,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -754,39 +856,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="5"/>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="5"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="5"/>
     </row>
@@ -822,509 +924,509 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13">
         <v>44995.0</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H2" s="15"/>
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="13">
         <v>44994.0</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H3" s="15"/>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="13">
         <v>44994.0</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H4" s="15"/>
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="19">
         <v>44996.0</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="19">
         <v>44996.0</v>
       </c>
       <c r="G6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="16" t="s">
         <v>36</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="19">
         <v>44996.0</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H7" s="21"/>
     </row>
     <row r="8">
       <c r="A8" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="19">
         <v>44997.0</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H8" s="21"/>
     </row>
     <row r="9">
       <c r="A9" s="22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="25">
         <v>44997.0</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H9" s="27"/>
     </row>
     <row r="10">
       <c r="A10" s="28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="31">
         <v>44994.0</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B11" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="28" t="s">
-        <v>48</v>
-      </c>
       <c r="D11" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E11" s="33"/>
       <c r="F11" s="31">
         <v>44999.0</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="31">
         <v>45000.0</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E13" s="24"/>
       <c r="F13" s="25">
         <v>45001.0</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H13" s="27"/>
     </row>
     <row r="14">
       <c r="A14" s="28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="31">
         <v>45001.0</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H14" s="28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="31">
         <v>45002.0</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="28"/>
       <c r="B16" s="34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="31">
         <v>45003.0</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="25">
         <v>45004.0</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H17" s="27"/>
     </row>
     <row r="18">
       <c r="A18" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="25">
         <v>45004.0</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="36" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E19" s="39"/>
       <c r="F19" s="40">
         <v>45005.0</v>
       </c>
       <c r="G19" s="41" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H19" s="36" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E20" s="39"/>
       <c r="F20" s="40">
         <v>45006.0</v>
       </c>
       <c r="G20" s="41" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H20" s="36" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E21" s="24"/>
       <c r="F21" s="25">
         <v>45006.0</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H21" s="27"/>
     </row>
     <row r="22">
       <c r="A22" s="36" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E22" s="39"/>
       <c r="F22" s="40">
         <v>45007.0</v>
       </c>
       <c r="G22" s="41" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H22" s="42"/>
     </row>
@@ -8203,4 +8305,208 @@
   </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="18.63"/>
+    <col customWidth="1" min="3" max="3" width="9.75"/>
+    <col customWidth="1" min="5" max="5" width="14.38"/>
+    <col customWidth="1" min="6" max="6" width="8.38"/>
+    <col customWidth="1" min="8" max="8" width="14.13"/>
+    <col customWidth="1" min="9" max="9" width="8.38"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="E2" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="46"/>
+      <c r="H2" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" s="46"/>
+    </row>
+    <row r="3">
+      <c r="B3" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="E6" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="46"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="46"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E10:F10"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>